<commit_message>
changes after Cursor recommendations
</commit_message>
<xml_diff>
--- a/Platform_Qualifier/data/Platform_Qualification_Result.xlsx
+++ b/Platform_Qualifier/data/Platform_Qualification_Result.xlsx
@@ -2,14 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Qualification-Checklist" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="181029" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -18,10 +19,10 @@
   <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
-      <sz val="12"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -49,9 +50,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -134,44 +135,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -198,32 +199,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -250,24 +233,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -279,162 +244,166 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="phClr"/>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
@@ -444,46 +413,69 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A13:F36"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
-    <row r="27"/>
-    <row r="28"/>
-    <row r="29"/>
-    <row r="30"/>
-    <row r="31"/>
-    <row r="33">
-      <c r="F33" t="n">
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Criterion</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Question</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Weighted Score</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Justification</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="36">
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>Project classified as: Application Development</t>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Classification</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Application Development</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes after excel name changes and first working code including chunk length, model changes for temp etc
</commit_message>
<xml_diff>
--- a/Platform_Qualifier/data/Platform_Qualification_Result.xlsx
+++ b/Platform_Qualifier/data/Platform_Qualification_Result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,25 +453,716 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Scope &amp; Reusability</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Does the solution provide reusable frameworks, services, or APIs that multiple teams/apps can build upon?</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>30</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Answer: Yes, the solution provides reusable frameworks, services, or APIs that multiple teams/apps can build upon. The solution leverages microservices architecture and design patterns to provide a modular and extensible framework for building various applications and services. This allows multiple teams to build upon the same set of components and services</t>
+        </is>
+      </c>
+    </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Total</t>
-        </is>
+          <t>Ecosystem Enablement</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Can third parties or internal users build on top of the platform (not just consume it)?</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>30</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>120</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>The BRD/Scope document outlines several non-functional requirements related to development, testing, and deployment. These include timelines for developing specifications, supporting 2-week sprints, and completing rigorous acceptance tests with the ATEL business and</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Multi-Use-Case Support</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Can the platform support multiple apps/use cases from the same foundation?</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>25</v>
+      </c>
+      <c r="E4" t="n">
+        <v>75</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Yes, the platform can support multiple apps/use cases from the same foundation. The vendor should provide a lean named team and take required ARB approvals before starting development work. Additionally, the vendor should provide automated daily backups, point-in-time recovery,</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Scalability &amp; Resilience</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Is there a requirement for 
+the platform to scale to support
+ increasing users, applications, or data 
+volumes while maintaining resilience?
+Will the platform scale to thousands of tenants, millions of requests, with built-in HA/failover?</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>25</v>
+      </c>
+      <c r="E5" t="n">
+        <v>100</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Yes, there is a requirement for the platform to scale to support increasing users, applications, or data volumes while maintaining resilience. The BRD mentions that the platform should be easily scalable from 500 to 10,000 chargers</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Multi-Tenant / Shared Model</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Does it support secure, isolated use by multiple tenants or customers on shared infra?</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>20</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Answer: Yes, the proposed solution supports secure and isolated use by multiple tenants or customers on shared infrastructure. The solution will be designed to provide separate and isolated environments for each tenant or customer, ensuring that their data and applications are secure and not accessible to other tenants or customers. This will be achieved</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Interoperability</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Does it need to integrate with external or internal systems via APIs, connectors, etc.?</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" t="n">
+        <v>20</v>
+      </c>
+      <c r="E7" t="n">
+        <v>60</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>The system requires integration with external and internal systems via APIs, connectors, and other integration methods to function effectively. Here are some of the integrations required:</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Migration Readiness</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Does scope involve infra transformation like cloud migration or replatforming?</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="n">
+        <v>20</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Answer: No, the scope of this RFP does not involve infrastructure transformation such as cloud migration or replatforming. The focus is on developing and implementing a Charge Point Management Software (CPMS) for Adani TotalEnergies E-Mobility Ltd.'s electric mobility operations. The</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Observability &amp; Telemetry</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Are metrics, logs, traces, and dashboards required for platform visibility?</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" t="n">
+        <v>20</v>
+      </c>
+      <c r="E9" t="n">
+        <v>60</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>The BRD/Scope document outlines the non-functional requirements for the development of Adani's CPMS platform. These include metrics, logs, traces,</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Extensible APIs &amp; Webhooks</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Does the platform expose APIs, SDKs, or webhooks for extensions or automation?</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" t="n">
+        <v>20</v>
+      </c>
+      <c r="E10" t="n">
+        <v>60</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>The BRD document mentions that the platform will have APIs, SDKs, and webhooks for extensions or automation. This means that developers can</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Developer Experience</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Is the platform designed for internal or external developers to self-serve efficiently?</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>3</v>
+      </c>
+      <c r="D11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E11" t="n">
+        <v>60</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>The BRD/Scope document outlines the requirements for the platform, including the non-functional requirements such as development, testing, and deployment timelines. The document also</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Security &amp; Compliance</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Must the platform provide shared security features for built-on apps?</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>3</v>
+      </c>
+      <c r="D12" t="n">
+        <v>20</v>
+      </c>
+      <c r="E12" t="n">
+        <v>60</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>The platform must provide shared security features for built-on apps to ensure the safety and privacy of users' data. This includes features such as authentication, authorization, data encryption, and access control. By providing these features, the platform can prevent unauthorized access to sensitive</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Cross-Domain Applicability</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Is it usable across different business units or domains?</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" t="n">
+        <v>15</v>
+      </c>
+      <c r="E13" t="n">
+        <v>45</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>The document appears to be a comprehensive list of features and functionalities for an EV charging platform. It covers various aspects such as user management, transaction tracking, reporting, and charge control. The document also mentions the importance of customization and scalability, indicating that it</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Customer's Business Model</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Is the solution aligned with a SaaS/ISV model (sold or licensed for building on top)?</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" t="n">
+        <v>15</v>
+      </c>
+      <c r="E14" t="n">
+        <v>45</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>The document outlines the functional and technical requirements for a CPMS solution to manage Adani TotalEnergies E-Mobility Limited's (ATEL) vast charging infrastructure. The proposed solution is designed as a SaaS/ISV model,</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Flexibility &amp; Customization</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Does the system need to 
+be highly flexible and 
+customizable to meet 
+varying customer requirements?</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>15</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Answer: Yes, the system needs to be highly flexible and customizable to meet varying customer requirements. The OCPP is designed to manage charging infrastructure for electric vehicles (EVs) across various locations, including residential areas, commercial spaces, and public parking lots. As such, it must be able</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Ease of Use/
+Ease of onboarding</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Can new developers/customers 
+get started in minutes via 
+docs, CLI, quickstarts, 
+sandbox?</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>4</v>
+      </c>
+      <c r="D16" t="n">
+        <v>15</v>
+      </c>
+      <c r="E16" t="n">
+        <v>60</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>The document provides a comprehensive list of functional and non-functional requirements for the development of an e-mobility platform. The emphasis on scalability, reliability, security, and ease of use suggests that the platform will be designed with a focus on us</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Governance &amp; Policy</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Are controls needed to enforce compliance, access, and usage across tenants?</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" t="n">
+        <v>15</v>
+      </c>
+      <c r="E17" t="n">
+        <v>45</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>A multi-tenant platform requires controls to ensure each tenant's data and resources are secure and isolated from other tenants. These controls can include:</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Upgradeability &amp; Versioning</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Does it require backward-compatible upgrades and controlled deprecations?</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>3</v>
+      </c>
+      <c r="D18" t="n">
+        <v>10</v>
+      </c>
+      <c r="E18" t="n">
+        <v>30</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Answer: Yes, the RFP requires backward-compatible upgrades and controlled deprecations. Score: 3 Justification: The RFP explicitly states that the CPMS must be designed to accommodate future upgrades and controlled deprecations without disrupting operations or compromising security. This indicates that</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Abstracts Complexity</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Does the platform hide complex infra or workflows for dev/user simplicity?</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>3</v>
+      </c>
+      <c r="D19" t="n">
+        <v>10</v>
+      </c>
+      <c r="E19" t="n">
+        <v>30</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>The BRD/Scope document outlines various non-functional requirements related to development, testing, and deployment of the CPMS platform. These include timelines for developing specifications</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Standardization Enabler</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Will it help unify dev practices or architecture across teams?</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>23</v>
+      </c>
+      <c r="D20" t="n">
+        <v>10</v>
+      </c>
+      <c r="E20" t="n">
+        <v>230</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Score: 2-3
+The document provides a comprehensive set of functional and technical requirements for the CPMS, which can help unify dev practices or architecture across teams. Here are some reasons why:
+1. Standardized architecture: The document outlines a standardized architecture for the CPMS,</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Total Weighted Score:</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Total Weighted Score:</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>3</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Score: 3
+The weighted score is calculated by multiplying each criterion's weightage by the corresponding rating. Based on the provided information, the following is the weighted score for the given RFP:
+1. System Architecture (4 points): The proposed system architecture is comprehensive and</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Platform Qualification Interpretation</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Platform Qualification Interpretation</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>3</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>The question is asking for the interpretation of platform qualification, which is a critical aspect of any charging infrastructure. The OCPP (Open Charge Point Protocol) is a standardized communication protocol that enables charge points to communicate with electric vehicles and other charg</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Total Weighted Score Range</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Interpretation</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>3</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>The provided feature list covers a wide range of functionalities that are essential for an e-mobility platform. These features include user registration and login, charging station management, transaction management, reporting and analytics, marketplace integration, and certification requirements. Additionally,</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>0 – 300</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Minimal platform traits — likely a custom or point application</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Based on the information provided in the RFP, the platform is expected to have several key features and functionalities, including a mobile app for customers, online support documents, a network planning tool, and integration with external and internal systems. While it is possible that some of these</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>301 – 600</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Some reusable or multi-use elements — consider modularizing further</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>The document provides a comprehensive list of features for the customer web and mobile app, including login options, vehicle registration, current location plotting, filter options, and more. While some of these features may be reusable or modularizable, the current structure is well-</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>601 – 850</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>High platform potential — reusable, multi-tenant, some ecosystem signs</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>3</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>The high platform potential is evident in the solution proposed by the vendor. The use of a multi-tenant, reusable platform suggests that the solution can be easily adapted and deployed for different customers or use cases, which increases its potential value. Additionally, the vendor has shown</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>&gt; 850</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Fully qualified platform — reusable, extensible, scalable, ecosystem-ready</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>3</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>The BRD outlines the functional and non-functional requirements for the CPMS platform. The platform is expected to be developed on Adani's Azure cloud, with a development timeline of not more than 6 months. The vendor is expected to support 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
           <t>Classification</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Application Development</t>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Enterprise-grade Platform</t>
         </is>
       </c>
     </row>

</xml_diff>